<commit_message>
Add LDA, kNN, and SVM classification
</commit_message>
<xml_diff>
--- a/clinical_data/Final_BIMS.xlsx
+++ b/clinical_data/Final_BIMS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livejohnshopkins-my.sharepoint.com/personal/sbhatt15_jh_edu/Documents/Shubhayu_Projects/Johns Hopkins University/ICU Motion Study/bims/clinical_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="145" documentId="8_{E2057880-4088-4A1B-8C45-F723981FAB7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{05B41DEC-9163-4998-A44A-0726B2C61A09}"/>
+  <xr:revisionPtr revIDLastSave="151" documentId="8_{E2057880-4088-4A1B-8C45-F723981FAB7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EE93EDE7-6FB6-4F83-A83B-C3958EAF8C2D}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3FB8A694-FA0D-BD43-8E2A-E48847BF0EB3}"/>
   </bookViews>
@@ -1585,9 +1585,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD2E54B0-F388-8644-8F07-ED4C651001CA}">
   <dimension ref="A1:CP96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BD35" sqref="BD35"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R75" sqref="R75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -15225,30 +15225,6 @@
       <c r="CI74" s="53"/>
     </row>
     <row r="75" spans="1:94" x14ac:dyDescent="0.3">
-      <c r="M75" s="75">
-        <f>SUM(M4:M74)</f>
-        <v>11</v>
-      </c>
-      <c r="N75" s="75">
-        <f t="shared" ref="N75:R75" si="0">SUM(N4:N74)</f>
-        <v>20</v>
-      </c>
-      <c r="O75" s="75">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="P75" s="75">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="Q75" s="75">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="R75" s="75">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
       <c r="BJ75" s="27"/>
       <c r="BQ75" s="27"/>
     </row>

</xml_diff>

<commit_message>
changes to classification and stratified CV
</commit_message>
<xml_diff>
--- a/clinical_data/Final_BIMS.xlsx
+++ b/clinical_data/Final_BIMS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livejohnshopkins-my.sharepoint.com/personal/sbhatt15_jh_edu/Documents/Shubhayu_Projects/Johns Hopkins University/ICU Motion Study/bims/clinical_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="151" documentId="8_{E2057880-4088-4A1B-8C45-F723981FAB7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EE93EDE7-6FB6-4F83-A83B-C3958EAF8C2D}"/>
+  <xr:revisionPtr revIDLastSave="158" documentId="8_{E2057880-4088-4A1B-8C45-F723981FAB7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D8E313F2-3026-4F65-AD9E-A452D9BDA008}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3FB8A694-FA0D-BD43-8E2A-E48847BF0EB3}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Patient Data" sheetId="2" r:id="rId1"/>
     <sheet name="GOS-E" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1034,7 +1034,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1257,6 +1257,9 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1267,6 +1270,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1585,9 +1594,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD2E54B0-F388-8644-8F07-ED4C651001CA}">
   <dimension ref="A1:CP96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R75" sqref="R75"/>
+    <sheetView tabSelected="1" topLeftCell="BW1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="BZ78" sqref="BZ78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1700,20 +1709,20 @@
         <v>5</v>
       </c>
       <c r="H1" s="13"/>
-      <c r="I1" s="76" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="76"/>
-      <c r="K1" s="76"/>
+      <c r="I1" s="77" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
       <c r="L1" s="13"/>
-      <c r="M1" s="79" t="s">
+      <c r="M1" s="80" t="s">
         <v>267</v>
       </c>
-      <c r="N1" s="79"/>
-      <c r="O1" s="79"/>
-      <c r="P1" s="79"/>
-      <c r="Q1" s="79"/>
-      <c r="R1" s="79"/>
+      <c r="N1" s="80"/>
+      <c r="O1" s="80"/>
+      <c r="P1" s="80"/>
+      <c r="Q1" s="80"/>
+      <c r="R1" s="80"/>
       <c r="S1" s="13"/>
       <c r="T1" s="26" t="s">
         <v>7</v>
@@ -1723,66 +1732,66 @@
         <v>8</v>
       </c>
       <c r="W1" s="13"/>
-      <c r="X1" s="76" t="s">
+      <c r="X1" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="Y1" s="76"/>
+      <c r="Y1" s="77"/>
       <c r="Z1" s="13"/>
-      <c r="AA1" s="76" t="s">
+      <c r="AA1" s="77" t="s">
         <v>10</v>
       </c>
-      <c r="AB1" s="76"/>
-      <c r="AC1" s="76"/>
-      <c r="AD1" s="76"/>
+      <c r="AB1" s="77"/>
+      <c r="AC1" s="77"/>
+      <c r="AD1" s="77"/>
       <c r="AE1" s="13"/>
-      <c r="AF1" s="76" t="s">
+      <c r="AF1" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="AG1" s="76"/>
+      <c r="AG1" s="77"/>
       <c r="AH1" s="13"/>
-      <c r="AI1" s="77" t="s">
+      <c r="AI1" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="AJ1" s="77"/>
-      <c r="AK1" s="77"/>
-      <c r="AL1" s="77"/>
-      <c r="AM1" s="77"/>
-      <c r="AN1" s="77"/>
-      <c r="AO1" s="77"/>
-      <c r="AP1" s="77"/>
+      <c r="AJ1" s="78"/>
+      <c r="AK1" s="78"/>
+      <c r="AL1" s="78"/>
+      <c r="AM1" s="78"/>
+      <c r="AN1" s="78"/>
+      <c r="AO1" s="78"/>
+      <c r="AP1" s="78"/>
       <c r="AQ1" s="12"/>
-      <c r="AR1" s="77" t="s">
+      <c r="AR1" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="AS1" s="77"/>
-      <c r="AT1" s="77"/>
-      <c r="AU1" s="77"/>
-      <c r="AV1" s="77"/>
-      <c r="AW1" s="77"/>
-      <c r="AX1" s="77"/>
-      <c r="AY1" s="77"/>
+      <c r="AS1" s="78"/>
+      <c r="AT1" s="78"/>
+      <c r="AU1" s="78"/>
+      <c r="AV1" s="78"/>
+      <c r="AW1" s="78"/>
+      <c r="AX1" s="78"/>
+      <c r="AY1" s="78"/>
       <c r="AZ1" s="12"/>
-      <c r="BA1" s="76" t="s">
+      <c r="BA1" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="BB1" s="76"/>
-      <c r="BC1" s="76"/>
-      <c r="BD1" s="76"/>
-      <c r="BE1" s="76"/>
-      <c r="BF1" s="76"/>
-      <c r="BG1" s="76"/>
-      <c r="BH1" s="76"/>
+      <c r="BB1" s="77"/>
+      <c r="BC1" s="77"/>
+      <c r="BD1" s="77"/>
+      <c r="BE1" s="77"/>
+      <c r="BF1" s="77"/>
+      <c r="BG1" s="77"/>
+      <c r="BH1" s="77"/>
       <c r="BI1" s="13"/>
-      <c r="BJ1" s="76" t="s">
+      <c r="BJ1" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="BK1" s="76"/>
-      <c r="BL1" s="76"/>
-      <c r="BM1" s="76"/>
-      <c r="BN1" s="76"/>
-      <c r="BO1" s="76"/>
-      <c r="BP1" s="76"/>
-      <c r="BQ1" s="76"/>
+      <c r="BK1" s="77"/>
+      <c r="BL1" s="77"/>
+      <c r="BM1" s="77"/>
+      <c r="BN1" s="77"/>
+      <c r="BO1" s="77"/>
+      <c r="BP1" s="77"/>
+      <c r="BQ1" s="77"/>
       <c r="BR1" s="12"/>
       <c r="BS1" s="26" t="s">
         <v>16</v>
@@ -1792,17 +1801,17 @@
         <v>17</v>
       </c>
       <c r="BV1" s="13"/>
-      <c r="BW1" s="76" t="s">
+      <c r="BW1" s="77" t="s">
         <v>18</v>
       </c>
-      <c r="BX1" s="76"/>
+      <c r="BX1" s="77"/>
       <c r="BZ1" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="CB1" s="76" t="s">
+      <c r="CB1" s="77" t="s">
         <v>20</v>
       </c>
-      <c r="CC1" s="76"/>
+      <c r="CC1" s="77"/>
       <c r="CE1" s="26" t="s">
         <v>21</v>
       </c>
@@ -1862,14 +1871,14 @@
         <v>25</v>
       </c>
       <c r="Z2" s="9"/>
-      <c r="AA2" s="78" t="s">
+      <c r="AA2" s="79" t="s">
         <v>26</v>
       </c>
-      <c r="AB2" s="78"/>
-      <c r="AC2" s="78" t="s">
+      <c r="AB2" s="79"/>
+      <c r="AC2" s="79" t="s">
         <v>27</v>
       </c>
-      <c r="AD2" s="78"/>
+      <c r="AD2" s="79"/>
       <c r="AE2" s="9"/>
       <c r="AF2" s="27" t="s">
         <v>28</v>
@@ -4318,7 +4327,7 @@
       <c r="CC14" s="52">
         <v>0</v>
       </c>
-      <c r="CE14" s="50">
+      <c r="CE14" s="82">
         <v>1</v>
       </c>
       <c r="CG14" s="47">
@@ -5522,11 +5531,12 @@
       <c r="CC20" s="43">
         <v>0.1</v>
       </c>
-      <c r="CE20" s="53">
-        <v>4</v>
-      </c>
-      <c r="CG20" s="53">
-        <v>1</v>
+      <c r="CE20" s="81">
+        <v>4</v>
+      </c>
+      <c r="CF20" s="76"/>
+      <c r="CG20" s="81">
+        <v>0</v>
       </c>
       <c r="CI20" s="53"/>
     </row>
@@ -6906,11 +6916,12 @@
       <c r="CC27" s="43">
         <v>0.95</v>
       </c>
-      <c r="CE27" s="53">
+      <c r="CE27" s="81">
         <v>7</v>
       </c>
-      <c r="CG27" s="53">
-        <v>1</v>
+      <c r="CF27" s="76"/>
+      <c r="CG27" s="81">
+        <v>0</v>
       </c>
       <c r="CI27" s="53"/>
     </row>

</xml_diff>